<commit_message>
I learned how to Graphics
</commit_message>
<xml_diff>
--- a/Excel lessons.xlsx
+++ b/Excel lessons.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27804"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2FA1C2D-AAD0-4AF6-B884-14D75275B7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55139\Documents\GitHub\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2044D586-80BD-4921-8FBB-F76340C0CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8325" yWindow="-15000" windowWidth="17460" windowHeight="13350" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Functions" sheetId="1" r:id="rId1"/>
@@ -13,22 +18,12 @@
     <sheet name="Conditionals Functions" sheetId="3" r:id="rId3"/>
     <sheet name="Concatenate" sheetId="4" r:id="rId4"/>
     <sheet name="Conditional Formatting" sheetId="5" r:id="rId5"/>
+    <sheet name="Graphics" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -42,7 +37,15 @@
   <commentList>
     <comment ref="H4" authorId="0" shapeId="0" xr:uid="{8D0D2EE1-8F45-48B0-9C6E-50239A3E62D0}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     WHATS THE DIFFERENCE BETWEEN FUNCTIONS AND FORMULAS?
@@ -51,6 +54,7 @@
   ex: =sum, =concat ...
 FORMULA:
 Like a personalized scrip that you own make and can use one or more functions together</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -65,13 +69,22 @@
   <commentList>
     <comment ref="E4" authorId="0" shapeId="0" xr:uid="{83879869-AE6A-4DE9-BEC3-4103D3362A77}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     ABSOLUTE REFERENCE
 USE "$" TO FROZE IT.
 $G = it froze the column;
 $4 = it froze the line.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -79,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
   <si>
     <t>Using Basic Funtions</t>
   </si>
@@ -220,6 +233,33 @@
   </si>
   <si>
     <t>Problem: Which values are ABOVE AVERAGE?</t>
+  </si>
+  <si>
+    <t>Making Graphics</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Guilherme</t>
+  </si>
+  <si>
+    <t>Pamela</t>
+  </si>
+  <si>
+    <t>Matheus</t>
+  </si>
+  <si>
+    <t>Maykon</t>
+  </si>
+  <si>
+    <t>Angela</t>
   </si>
 </sst>
 </file>
@@ -241,14 +281,14 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -395,7 +435,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -436,19 +476,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -474,10 +530,2098 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Age</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphics!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Age</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphics!$B$4:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Angela</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Guilherme</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pamela</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Matheus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maykon</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphics!$C$4:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-872F-488C-992D-2E84DDC093BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="183050048"/>
+        <c:axId val="183052128"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="183050048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="183052128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="183052128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="183050048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" b="1"/>
+              <a:t>Resultado das</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" b="1" baseline="0"/>
+              <a:t> Notas</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphics!$B$15:$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Angela</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Guilherme</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pamela</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Matheus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maykon</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphics!$C$15:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7295-419B-9E28-B3965C5D0E09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphics!$B$15:$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Angela</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Guilherme</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pamela</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Matheus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maykon</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphics!$D$15:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7295-419B-9E28-B3965C5D0E09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16307830271216098"/>
+          <c:y val="0.8524300087489064"/>
+          <c:w val="0.70717672790901143"/>
+          <c:h val="0.11979221347331584"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9B5EFF6-5E13-4820-A953-F33FDB24469A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D4C65FE-54AC-4D96-893B-C6B7246F06C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="guilherme teixeira" id="{116C0750-AA2F-41C5-8B2E-71EB639AE745}" userId="9a3f381fadf300f8" providerId="Windows Live"/>
 </personList>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EEF84849-01DF-4156-8CEB-DF70E829968A}" name="Table1" displayName="Table1" ref="B3:C8" totalsRowShown="0">
+  <autoFilter ref="B3:C8" xr:uid="{EEF84849-01DF-4156-8CEB-DF70E829968A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C8">
+    <sortCondition descending="1" ref="C3:C8"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{0CD02F1B-5075-4043-A0BF-B4ABD0F1E8DD}" name="Student" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{3EF91C04-9ECB-489E-A93B-0CAECCB90A8D}" name="Age" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2BC69DDB-5844-4F24-A26F-FB0C11AC4C1C}" name="Table13" displayName="Table13" ref="B14:D19" totalsRowShown="0">
+  <autoFilter ref="B14:D19" xr:uid="{2BC69DDB-5844-4F24-A26F-FB0C11AC4C1C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:C19">
+    <sortCondition descending="1" ref="C3:C8"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{4B0A0008-8BE9-400E-B2A4-289965EF189B}" name="Student" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{93330ECC-6E8D-411F-9FCC-DEBD45AEDD10}" name="Age" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{53CEF673-3975-45A8-82EA-5DEC97D0CD17}" name="Note"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -827,10 +2971,10 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="7" max="7" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="15" customFormat="1" ht="19.5">
@@ -854,7 +2998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="15">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -875,7 +3019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="15">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -893,7 +3037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="15">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -911,7 +3055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="15">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -929,7 +3073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="15">
       <c r="E8" s="9" t="s">
         <v>16</v>
       </c>
@@ -941,7 +3085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="15">
       <c r="E9" s="9" t="s">
         <v>18</v>
       </c>
@@ -953,7 +3097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="15">
       <c r="E10" s="11" t="s">
         <v>20</v>
       </c>
@@ -979,12 +3123,12 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" s="15" customFormat="1" ht="19.5">
@@ -1003,7 +3147,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" ht="15">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1075,12 +3219,12 @@
       <selection activeCell="B4" sqref="B4:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="10.375" customWidth="1"/>
+    <col min="7" max="7" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="15" customFormat="1" ht="19.5">
@@ -1088,22 +3232,22 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="17.25">
+    <row r="3" spans="2:9" ht="16.5">
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" ht="15">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +3267,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" ht="15">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +3283,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" ht="15">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1158,7 +3302,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" ht="15">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +3318,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" ht="15">
       <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1212,7 +3356,7 @@
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="2:9" ht="17.25">
+    <row r="11" spans="2:9" ht="16.5">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1220,15 +3364,15 @@
         <v>646</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" ht="15">
       <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
@@ -1247,7 +3391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" ht="15">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1263,7 +3407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" ht="15">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1279,7 +3423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" ht="15">
       <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1295,7 +3439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" ht="15">
       <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
@@ -1356,7 +3500,7 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
@@ -1366,7 +3510,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" ht="15">
       <c r="B3" s="23" t="s">
         <v>36</v>
       </c>
@@ -1393,7 +3537,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" ht="15">
       <c r="B8" s="23" t="s">
         <v>41</v>
       </c>
@@ -1403,7 +3547,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" ht="15">
       <c r="B11" s="23" t="s">
         <v>43</v>
       </c>
@@ -1423,13 +3567,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBB8A02-6A94-45CB-97CF-D01268BBEEF3}">
   <dimension ref="B1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="15" customFormat="1" ht="19.5">
@@ -1437,22 +3581,22 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="18.75">
+    <row r="3" spans="2:5" ht="18">
       <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="25">
         <v>1</v>
       </c>
     </row>
@@ -1579,8 +3723,153 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C18">
-    <cfRule type="aboveAverage" dxfId="0" priority="1"/>
+    <cfRule type="aboveAverage" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA89FA6-D8C9-4107-AD92-C3DE04CE0800}">
+  <dimension ref="B1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="21.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" style="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" s="15" customFormat="1" ht="20.25" thickBot="1">
+      <c r="B1" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="2" spans="2:4" ht="15" thickTop="1"/>
+    <row r="3" spans="2:4">
+      <c r="B3" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="29">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="29">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="29">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="29">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="29">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="29">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>